<commit_message>
Update Day 1 Practice at Home.xlsx
</commit_message>
<xml_diff>
--- a/Day 1 Practice at Home.xlsx
+++ b/Day 1 Practice at Home.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IRC\Testing and Automation\Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation and Testing\AutomationTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{086F2F3C-B241-4C2D-9EEE-C31D8BB21B66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1E22E4-0BAC-42C4-BD09-3E076A1B7C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{7B17EDA8-F7E7-42F4-BD5F-B5BF10E31CC2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7B17EDA8-F7E7-42F4-BD5F-B5BF10E31CC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="92">
   <si>
     <t>TestID</t>
   </si>
@@ -156,10 +156,6 @@
 3.Admin is able to click add doctor button.</t>
   </si>
   <si>
-    <t>Admin login ID : admin 
-Admin password : Test@12347</t>
-  </si>
-  <si>
     <t>Admin able to click add doctor button.</t>
   </si>
   <si>
@@ -172,13 +168,181 @@
     <t>1.Admin is logged in.
 2.Admin is in admin dashboard.
 3.Admin is able to click add doctor button.                                                                   4.Form is displayed</t>
+  </si>
+  <si>
+    <t>TC 2.5</t>
+  </si>
+  <si>
+    <t>Admin fills the form completely.</t>
+  </si>
+  <si>
+    <t>1.Admin is logged in.
+2.Admin is in admin dashboard.
+3.Admin is able to click add doctor button.
+4.Form is displayed.
+5.Details are filled in the form.</t>
+  </si>
+  <si>
+    <t>#Doctor Specialization : selected       #Doctor Name : Mayura                       #Doctor Clinic address : 10/78 , crosscut road,Hosur.                                       #Doctor consultancy fee : Rs 250         #Doctor contact number : 9862675687     #Doctor Email : drmayura@gmail.com     #Password : mayura1234                                    #Confirm password : mayura1234</t>
+  </si>
+  <si>
+    <t>Details form filled.</t>
+  </si>
+  <si>
+    <t>Details form displayed.</t>
+  </si>
+  <si>
+    <t>TC 2.6</t>
+  </si>
+  <si>
+    <t>TC 2.7</t>
+  </si>
+  <si>
+    <t>Admin fills the form completely and criteria should match and submit button enabled.</t>
+  </si>
+  <si>
+    <t>Fields are filled with proper criteria and submit button enabled.</t>
+  </si>
+  <si>
+    <t>Admin fills the form completely and clicks the submit button .</t>
+  </si>
+  <si>
+    <t>Doctor info added Successfully.</t>
+  </si>
+  <si>
+    <t>TC 2.8</t>
+  </si>
+  <si>
+    <t>Success message displayed institute details should be displayed on the doctor page.</t>
+  </si>
+  <si>
+    <t>1.Admin is logged in.
+2.Admin is in admin dashboard.
+3.Admin is able to click add doctor button.
+4.Form is displayed.
+5.Details are filled in the form.             6.Admin clicks the submit button.</t>
+  </si>
+  <si>
+    <t>Institute details displayed.</t>
+  </si>
+  <si>
+    <t>TC 3.1</t>
+  </si>
+  <si>
+    <t>To manage user details to update information.</t>
+  </si>
+  <si>
+    <t>TC 3.2</t>
+  </si>
+  <si>
+    <t>TC 3.3</t>
+  </si>
+  <si>
+    <t>Admin is able to click Manage users.</t>
+  </si>
+  <si>
+    <t>1.Admin is logged in.
+2.Admin is in admin dashboard.
+3.Admin is able to click manage users button.</t>
+  </si>
+  <si>
+    <t>Admin able to click  manage user button.</t>
+  </si>
+  <si>
+    <t>TC 3.4</t>
+  </si>
+  <si>
+    <t>Admin clicks the delete icon ,pop up alert displayed.</t>
+  </si>
+  <si>
+    <t>1.Admin is logged in.
+2.Admin is in admin dashboard.
+3.Admin is able to click manage users button.                                                                 4.Admin clicks delete icon</t>
+  </si>
+  <si>
+    <t>Pop up alert should be displayed as Are You sure you want to delete? And user details should be deleted.</t>
+  </si>
+  <si>
+    <t>TC 4.1</t>
+  </si>
+  <si>
+    <t>TC 4.2</t>
+  </si>
+  <si>
+    <t>TC 4.3</t>
+  </si>
+  <si>
+    <t>To manage patients details to update information.</t>
+  </si>
+  <si>
+    <t>Admin is able to click Manage patient.</t>
+  </si>
+  <si>
+    <t>Admin able to click  manage patient button.</t>
+  </si>
+  <si>
+    <t>TC 4.4</t>
+  </si>
+  <si>
+    <t>Admin clicks view icon in patient.</t>
+  </si>
+  <si>
+    <t>1.Admin is logged in.
+2.Admin is in admin dashboard.
+3.Admin is able to click manage patient button.</t>
+  </si>
+  <si>
+    <t>1.Admin is logged in.
+2.Admin is in admin dashboard.
+3.Admin is able to click manage patient button.                                                 4.Admin clicks view icon.</t>
+  </si>
+  <si>
+    <t>Admin clicks view icon.</t>
+  </si>
+  <si>
+    <t>TC 5.1</t>
+  </si>
+  <si>
+    <t>Admin wants to look at appointment history</t>
+  </si>
+  <si>
+    <t>TC 5.2</t>
+  </si>
+  <si>
+    <t>TC 5.3</t>
+  </si>
+  <si>
+    <t>Admin clicks appointment history and appointment history displayed.</t>
+  </si>
+  <si>
+    <t>1.Admin is logged in.
+2.Admin is in admin dashboard.
+3.Admin is able to click appointment history.</t>
+  </si>
+  <si>
+    <t>Appointment history displayed.</t>
+  </si>
+  <si>
+    <t>TEST CASE 5</t>
+  </si>
+  <si>
+    <t>TEST CASE 4</t>
+  </si>
+  <si>
+    <t>TEST CASE 3</t>
+  </si>
+  <si>
+    <t>TEST CASE 2</t>
+  </si>
+  <si>
+    <t>TEST CASE 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,15 +351,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -221,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -229,7 +408,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,140 +725,131 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A7E08A5-3F6E-4D23-98F2-ED1035E1DE29}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="41" customWidth="1"/>
     <col min="3" max="3" width="30.88671875" customWidth="1"/>
-    <col min="4" max="4" width="29.5546875" customWidth="1"/>
+    <col min="4" max="4" width="33.44140625" customWidth="1"/>
     <col min="5" max="5" width="24.109375" customWidth="1"/>
     <col min="6" max="6" width="20.5546875" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" s="5" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="2" spans="1:7" s="5" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="82.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="G6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="82.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>27</v>
@@ -689,56 +861,61 @@
         <v>24</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="G8" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>16</v>
@@ -746,40 +923,442 @@
     </row>
     <row r="11" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="139.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="B14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="141.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="139.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <mergeCells count="5">
+    <mergeCell ref="A28:XFD28"/>
+    <mergeCell ref="A23:XFD23"/>
+    <mergeCell ref="A18:XFD18"/>
+    <mergeCell ref="A9:XFD9"/>
+    <mergeCell ref="A3:XFD3"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>